<commit_message>
Major updates on the file readin gand writing parts
</commit_message>
<xml_diff>
--- a/SourceCompanyNames/SourceCompanyNames.xlsx
+++ b/SourceCompanyNames/SourceCompanyNames.xlsx
@@ -21,18 +21,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
   <si>
     <t xml:space="preserve">Coal India</t>
   </si>
   <si>
-    <t xml:space="preserve">Dabus India</t>
+    <t xml:space="preserve">Dabur India</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dalmia Bhara</t>
   </si>
   <si>
     <t xml:space="preserve">Infosys</t>
   </si>
   <si>
+    <t xml:space="preserve">KIOCL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Knitworth Export</t>
+  </si>
+  <si>
     <t xml:space="preserve">Maruti Suzuki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rites</t>
   </si>
   <si>
     <t xml:space="preserve">Infosys Ltd</t>
@@ -296,10 +308,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -326,6 +338,26 @@
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -357,267 +389,267 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>